<commit_message>
Deviation and coefficient of deviation exercises.
</commit_message>
<xml_diff>
--- a/resources/Part_3_Statistics/S15_L88/2.10.Standard-deviation-and-coefficient-of-variation-exercise.xlsx
+++ b/resources/Part_3_Statistics/S15_L88/2.10.Standard-deviation-and-coefficient-of-variation-exercise.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Iliya\Desktop\Statistics for Data Science and Business Analysis\Filming\Final excel\Section 2 - Descriptive statistics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\GitRepos\StatisticsBAandDS\DataScienceBootcamp\resources\Part_3_Statistics\S15_L88\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090"/>
   </bookViews>
   <sheets>
     <sheet name="Std and cv" sheetId="9" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Background</t>
   </si>
@@ -76,17 +76,52 @@
   </si>
   <si>
     <t>You have the annual personal income of 11 people from the USA and 10 from Denmark. You have the mean income for USA from previous exercises</t>
+  </si>
+  <si>
+    <t>Sample formulas</t>
+  </si>
+  <si>
+    <t>Mean DK</t>
+  </si>
+  <si>
+    <t>Copy:</t>
+  </si>
+  <si>
+    <t>distance</t>
+  </si>
+  <si>
+    <t>squared</t>
+  </si>
+  <si>
+    <t>Variance DK</t>
+  </si>
+  <si>
+    <t>Standard deviation US:</t>
+  </si>
+  <si>
+    <t>Standard deviation DK:</t>
+  </si>
+  <si>
+    <t>Coefficient of Variation US:</t>
+  </si>
+  <si>
+    <t>Coefficient of variation DK:</t>
+  </si>
+  <si>
+    <t>Task 3:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;\²\ * #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(\€\²\ * #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="6">
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;\²\ * #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_(\€\²\ * #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -158,9 +193,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -168,24 +203,26 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -497,44 +534,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:L26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.77734375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.33203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="23.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="5.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="2:12" ht="12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="2:12" ht="12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
@@ -542,7 +579,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
@@ -550,7 +587,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
@@ -558,13 +595,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B7" s="4"/>
       <c r="D7" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
         <v>3</v>
       </c>
@@ -572,7 +609,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
@@ -580,13 +617,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B10" s="4"/>
     </row>
-    <row r="11" spans="2:12" ht="12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B11" s="4"/>
     </row>
-    <row r="13" spans="2:12" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:12" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>6</v>
       </c>
@@ -601,8 +638,11 @@
         <f>AVERAGE(B14:B24)</f>
         <v>189848.18181818182</v>
       </c>
-    </row>
-    <row r="14" spans="2:12" ht="12" x14ac:dyDescent="0.25">
+      <c r="K13" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B14" s="5">
         <v>62000</v>
       </c>
@@ -626,9 +666,22 @@
         <v>63000</v>
       </c>
       <c r="F15" s="12"/>
-      <c r="H15" s="8"/>
-    </row>
-    <row r="16" spans="2:12" ht="12" x14ac:dyDescent="0.25">
+      <c r="H15" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" s="1">
+        <f>I14^(1/2)</f>
+        <v>365285.38095078978</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L15" s="19">
+        <f>I15/I13</f>
+        <v>1.9240920690018759</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B16" s="5">
         <v>49000</v>
       </c>
@@ -636,11 +689,16 @@
         <v>76000</v>
       </c>
       <c r="F16" s="12"/>
-      <c r="G16" s="7"/>
+      <c r="G16" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="K16" s="4"/>
       <c r="L16" s="16"/>
     </row>
-    <row r="17" spans="2:12" ht="12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B17" s="5">
         <v>324000</v>
       </c>
@@ -648,10 +706,20 @@
         <v>79000</v>
       </c>
       <c r="F17" s="12"/>
+      <c r="G17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="1">
+        <f>SUM(E14:E24)/COUNT(E14:E24)</f>
+        <v>67636.363636363632</v>
+      </c>
       <c r="K17" s="4"/>
       <c r="L17" s="17"/>
     </row>
-    <row r="18" spans="2:12" ht="12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B18" s="5">
         <v>1264000</v>
       </c>
@@ -659,12 +727,17 @@
         <v>67000</v>
       </c>
       <c r="F18" s="12"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="5"/>
+      <c r="H18" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I18" s="5">
+        <f>G39/(COUNT(E14:E24)-1)</f>
+        <v>37654545.454545453</v>
+      </c>
       <c r="K18" s="4"/>
       <c r="L18" s="16"/>
     </row>
-    <row r="19" spans="2:12" ht="12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B19" s="5">
         <v>54330</v>
       </c>
@@ -673,8 +746,22 @@
         <v>66000</v>
       </c>
       <c r="F19" s="12"/>
-    </row>
-    <row r="20" spans="2:12" ht="12" x14ac:dyDescent="0.25">
+      <c r="H19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" s="1">
+        <f>I18^(1/2)</f>
+        <v>6136.3299662375921</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L19" s="1">
+        <f>I19/I17</f>
+        <v>9.072530864060957E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B20" s="5">
         <v>64000</v>
       </c>
@@ -699,7 +786,7 @@
       </c>
       <c r="F21" s="12"/>
     </row>
-    <row r="22" spans="2:12" ht="12" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B22" s="5">
         <v>55000</v>
       </c>
@@ -720,7 +807,7 @@
       </c>
       <c r="F23" s="12"/>
     </row>
-    <row r="24" spans="2:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="6">
         <v>53000</v>
       </c>
@@ -733,11 +820,187 @@
     <row r="25" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B25" s="9"/>
     </row>
-    <row r="26" spans="2:12" ht="12" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
       <c r="H26" s="4"/>
       <c r="I26" s="12"/>
       <c r="K26" s="4"/>
       <c r="L26" s="16"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="E27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="E28" s="14">
+        <v>62000</v>
+      </c>
+      <c r="F28" s="18">
+        <f>E28-$I$17</f>
+        <v>-5636.3636363636324</v>
+      </c>
+      <c r="G28" s="18">
+        <f>F28^2</f>
+        <v>31768595.041322269</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="E29" s="14">
+        <v>63000</v>
+      </c>
+      <c r="F29" s="18">
+        <f t="shared" ref="F29:G38" si="0">E29-$I$17</f>
+        <v>-4636.3636363636324</v>
+      </c>
+      <c r="G29" s="18">
+        <f t="shared" ref="G29:G38" si="1">F29^2</f>
+        <v>21495867.768595006</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="E30" s="14">
+        <v>76000</v>
+      </c>
+      <c r="F30" s="18">
+        <f t="shared" si="0"/>
+        <v>8363.6363636363676</v>
+      </c>
+      <c r="G30" s="18">
+        <f t="shared" si="1"/>
+        <v>69950413.223140568</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="E31" s="14">
+        <v>79000</v>
+      </c>
+      <c r="F31" s="18">
+        <f t="shared" si="0"/>
+        <v>11363.636363636368</v>
+      </c>
+      <c r="G31" s="18">
+        <f t="shared" si="1"/>
+        <v>129132231.40495877</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="E32" s="14">
+        <v>67000</v>
+      </c>
+      <c r="F32" s="18">
+        <f t="shared" si="0"/>
+        <v>-636.36363636363239</v>
+      </c>
+      <c r="G32" s="18">
+        <f t="shared" si="1"/>
+        <v>404958.67768594535</v>
+      </c>
+    </row>
+    <row r="33" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E33" s="14">
+        <v>66000</v>
+      </c>
+      <c r="F33" s="18">
+        <f t="shared" si="0"/>
+        <v>-1636.3636363636324</v>
+      </c>
+      <c r="G33" s="18">
+        <f t="shared" si="1"/>
+        <v>2677685.9504132103</v>
+      </c>
+    </row>
+    <row r="34" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E34" s="14">
+        <v>69000</v>
+      </c>
+      <c r="F34" s="18">
+        <f t="shared" si="0"/>
+        <v>1363.6363636363676</v>
+      </c>
+      <c r="G34" s="18">
+        <f t="shared" si="1"/>
+        <v>1859504.1322314157</v>
+      </c>
+    </row>
+    <row r="35" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E35" s="14">
+        <v>68000</v>
+      </c>
+      <c r="F35" s="18">
+        <f t="shared" si="0"/>
+        <v>363.63636363636761</v>
+      </c>
+      <c r="G35" s="18">
+        <f t="shared" si="1"/>
+        <v>132231.40495868056</v>
+      </c>
+    </row>
+    <row r="36" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E36" s="14">
+        <v>57000</v>
+      </c>
+      <c r="F36" s="18">
+        <f t="shared" si="0"/>
+        <v>-10636.363636363632</v>
+      </c>
+      <c r="G36" s="18">
+        <f t="shared" si="1"/>
+        <v>113132231.40495859</v>
+      </c>
+    </row>
+    <row r="37" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E37" s="14">
+        <v>70000</v>
+      </c>
+      <c r="F37" s="18">
+        <f t="shared" si="0"/>
+        <v>2363.6363636363676</v>
+      </c>
+      <c r="G37" s="18">
+        <f t="shared" si="1"/>
+        <v>5586776.8595041512</v>
+      </c>
+    </row>
+    <row r="38" spans="5:7" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E38" s="15">
+        <v>67000</v>
+      </c>
+      <c r="F38" s="18">
+        <f t="shared" si="0"/>
+        <v>-636.36363636363239</v>
+      </c>
+      <c r="G38" s="18">
+        <f t="shared" si="1"/>
+        <v>404958.67768594535</v>
+      </c>
+    </row>
+    <row r="39" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E39" s="16">
+        <f>SUM(E28:E38)</f>
+        <v>744000</v>
+      </c>
+      <c r="G39" s="18">
+        <f>SUM(G28:G38)</f>
+        <v>376545454.5454545</v>
+      </c>
+    </row>
+    <row r="40" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E40" s="1">
+        <f>COUNT(E14:E24)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E41" s="18">
+        <f>E39/E40</f>
+        <v>67636.363636363632</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>